<commit_message>
December version of gr4sp with new db and changes to validation and exploration files
</commit_message>
<xml_diff>
--- a/simulationData/1948_2019_CPI_historic_Australia.xlsx
+++ b/simulationData/1948_2019_CPI_historic_Australia.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\angel\Documents\GitHub\gr4sp\experiments\simulationData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{940397BB-C599-4C15-AE6B-B36D20535D98}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8542C5C5-820A-4FD1-A2BA-D9E6BEBC6F48}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4C3C364B-2581-4959-BC09-DE0E467F90C6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$L$1:$L$71</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -33,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Year</t>
   </si>
@@ -61,16 +64,21 @@
   <si>
     <t>median</t>
   </si>
+  <si>
+    <t>filter</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="4">
-    <numFmt numFmtId="168" formatCode="0.0%"/>
-    <numFmt numFmtId="169" formatCode="0.000%"/>
-    <numFmt numFmtId="170" formatCode="0.0000%"/>
-    <numFmt numFmtId="172" formatCode="0.0"/>
+  <numFmts count="6">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="0.0%"/>
+    <numFmt numFmtId="165" formatCode="0.000%"/>
+    <numFmt numFmtId="166" formatCode="0.0000%"/>
+    <numFmt numFmtId="167" formatCode="0.0"/>
+    <numFmt numFmtId="169" formatCode="_-* #,##0.0000_-;\-* #,##0.0000_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -119,25 +127,28 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
+    <cellStyle name="Comma" xfId="3" builtinId="3"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
@@ -454,16 +465,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F076D4E-19F4-4F36-8E74-8579A6445293}">
   <dimension ref="A1:L75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A45" sqref="A45:XFD45"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="L63" sqref="L63:L71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="8" max="8" width="9.140625" style="1"/>
+    <col min="8" max="8" width="112.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -485,11 +497,14 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2019</v>
       </c>
@@ -513,8 +528,11 @@
         <f>ABS(1-(F3/F2))</f>
         <v>1.56385751520417E-2</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2018</v>
       </c>
@@ -534,16 +552,19 @@
         <v>113.3</v>
       </c>
       <c r="G3" s="3"/>
-      <c r="H3" s="6">
-        <f t="shared" ref="H2:H65" si="0">ABS(1-(F3/F4))</f>
+      <c r="H3" s="3">
+        <f>ABS(1-(F3/F4))</f>
         <v>1.980198019801982E-2</v>
       </c>
-      <c r="I3" s="10">
+      <c r="I3" s="9">
         <f>F3*1.0198</f>
         <v>115.54334</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2017</v>
       </c>
@@ -564,11 +585,14 @@
       </c>
       <c r="G4" s="3"/>
       <c r="H4" s="1">
-        <f t="shared" si="0"/>
+        <f>ABS(1-(F4/F5))</f>
         <v>1.9266055045871422E-2</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L4">
+        <v>2.9985007496251548E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2016</v>
       </c>
@@ -589,11 +613,14 @@
       </c>
       <c r="G5" s="3"/>
       <c r="H5" s="1">
-        <f t="shared" si="0"/>
+        <f>ABS(1-(F5/F6))</f>
         <v>1.3011152416356975E-2</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L5" s="10">
+        <v>7.4738415545589909E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2015</v>
       </c>
@@ -614,11 +641,14 @@
       </c>
       <c r="G6" s="3"/>
       <c r="H6" s="1">
-        <f t="shared" si="0"/>
+        <f>ABS(1-(F6/F7))</f>
         <v>1.5094339622641506E-2</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L6">
+        <v>1.0118043844856706E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2014</v>
       </c>
@@ -639,11 +669,14 @@
       </c>
       <c r="G7" s="3"/>
       <c r="H7" s="1">
-        <f t="shared" si="0"/>
+        <f>ABS(1-(F7/F8))</f>
         <v>2.4154589371980784E-2</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L7">
+        <v>1.2820512820512997E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2013</v>
       </c>
@@ -664,11 +697,14 @@
       </c>
       <c r="G8" s="3"/>
       <c r="H8" s="1">
-        <f t="shared" si="0"/>
+        <f>ABS(1-(F8/F9))</f>
         <v>2.4752475247524774E-2</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L8">
+        <v>1.298701298701288E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2012</v>
       </c>
@@ -689,11 +725,14 @@
       </c>
       <c r="G9" s="3"/>
       <c r="H9" s="1">
-        <f t="shared" si="0"/>
+        <f>ABS(1-(F9/F10))</f>
         <v>1.7119838872104776E-2</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L9">
+        <v>1.3011152416356975E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2011</v>
       </c>
@@ -714,11 +753,14 @@
       </c>
       <c r="G10" s="3"/>
       <c r="H10" s="1">
-        <f t="shared" si="0"/>
+        <f>ABS(1-(F10/F11))</f>
         <v>3.3298647242455903E-2</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L10">
+        <v>1.4836795252225476E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2010</v>
       </c>
@@ -739,11 +781,14 @@
       </c>
       <c r="G11" s="3"/>
       <c r="H11" s="1">
-        <f t="shared" si="0"/>
+        <f>ABS(1-(F11/F12))</f>
         <v>2.8907922912205342E-2</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L11">
+        <v>1.5094339622641506E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2009</v>
       </c>
@@ -764,11 +809,14 @@
       </c>
       <c r="G12" s="3"/>
       <c r="H12" s="1">
-        <f t="shared" si="0"/>
+        <f>ABS(1-(F12/F13))</f>
         <v>1.7429193899782147E-2</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L12">
+        <v>1.538461538461533E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2008</v>
       </c>
@@ -789,11 +837,14 @@
       </c>
       <c r="G13" s="3"/>
       <c r="H13" s="1">
-        <f t="shared" si="0"/>
+        <f>ABS(1-(F13/F14))</f>
         <v>4.4368600682593851E-2</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L13">
+        <v>1.5625E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2007</v>
       </c>
@@ -814,11 +865,14 @@
       </c>
       <c r="G14" s="3"/>
       <c r="H14" s="1">
-        <f t="shared" si="0"/>
+        <f>ABS(1-(F14/F15))</f>
         <v>2.3282887077997749E-2</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L14">
+        <v>1.56385751520417E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2006</v>
       </c>
@@ -839,11 +893,14 @@
       </c>
       <c r="G15" s="3"/>
       <c r="H15" s="1">
-        <f t="shared" si="0"/>
+        <f>ABS(1-(F15/F16))</f>
         <v>3.4939759036144658E-2</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L15">
+        <v>1.6694490818029983E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2005</v>
       </c>
@@ -864,8 +921,11 @@
       </c>
       <c r="G16" s="3"/>
       <c r="H16" s="1">
-        <f t="shared" si="0"/>
+        <f>ABS(1-(F16/F17))</f>
         <v>2.7227722772277252E-2</v>
+      </c>
+      <c r="L16">
+        <v>1.7119838872104776E-2</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
@@ -889,8 +949,11 @@
       </c>
       <c r="G17" s="3"/>
       <c r="H17" s="1">
-        <f t="shared" si="0"/>
+        <f>ABS(1-(F17/F18))</f>
         <v>2.2784810126582178E-2</v>
+      </c>
+      <c r="L17">
+        <v>1.7429193899782147E-2</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
@@ -914,8 +977,11 @@
       </c>
       <c r="G18" s="3"/>
       <c r="H18" s="1">
-        <f t="shared" si="0"/>
+        <f>ABS(1-(F18/F19))</f>
         <v>2.730819245773719E-2</v>
+      </c>
+      <c r="L18">
+        <v>1.9266055045871422E-2</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
@@ -939,8 +1005,11 @@
       </c>
       <c r="G19" s="3"/>
       <c r="H19" s="1">
-        <f t="shared" si="0"/>
+        <f>ABS(1-(F19/F20))</f>
         <v>3.0831099195710587E-2</v>
+      </c>
+      <c r="L19">
+        <v>1.9704433497536922E-2</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
@@ -964,8 +1033,11 @@
       </c>
       <c r="G20" s="3"/>
       <c r="H20" s="1">
-        <f t="shared" si="0"/>
+        <f>ABS(1-(F20/F21))</f>
         <v>4.3356643356643243E-2</v>
+      </c>
+      <c r="L20">
+        <v>1.980198019801982E-2</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
@@ -989,8 +1061,11 @@
       </c>
       <c r="G21" s="3"/>
       <c r="H21" s="1">
-        <f t="shared" si="0"/>
+        <f>ABS(1-(F21/F22))</f>
         <v>4.5321637426900541E-2</v>
+      </c>
+      <c r="L21">
+        <v>2.2784810126582178E-2</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
@@ -1014,8 +1089,11 @@
       </c>
       <c r="G22" s="3"/>
       <c r="H22" s="1">
-        <f t="shared" si="0"/>
+        <f>ABS(1-(F22/F23))</f>
         <v>1.4836795252225476E-2</v>
+      </c>
+      <c r="L22">
+        <v>2.3282887077997749E-2</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
@@ -1039,10 +1117,12 @@
       </c>
       <c r="G23" s="3"/>
       <c r="H23" s="1">
-        <f t="shared" si="0"/>
+        <f>ABS(1-(F23/F24))</f>
         <v>7.4738415545589909E-3</v>
       </c>
-      <c r="L23" s="4"/>
+      <c r="L23">
+        <v>2.3809523809523725E-2</v>
+      </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24">
@@ -1065,8 +1145,11 @@
       </c>
       <c r="G24" s="3"/>
       <c r="H24" s="1">
-        <f t="shared" si="0"/>
+        <f>ABS(1-(F24/F25))</f>
         <v>2.9985007496251548E-3</v>
+      </c>
+      <c r="L24">
+        <v>2.4154589371980784E-2</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
@@ -1090,8 +1173,11 @@
       </c>
       <c r="G25" s="3"/>
       <c r="H25" s="1">
-        <f t="shared" si="0"/>
+        <f>ABS(1-(F25/F26))</f>
         <v>2.6153846153846194E-2</v>
+      </c>
+      <c r="L25">
+        <v>2.4752475247524774E-2</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
@@ -1115,8 +1201,11 @@
       </c>
       <c r="G26" s="3"/>
       <c r="H26" s="1">
-        <f t="shared" si="0"/>
+        <f>ABS(1-(F26/F27))</f>
         <v>4.6698872785829293E-2</v>
+      </c>
+      <c r="L26">
+        <v>2.5316455696202445E-2</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
@@ -1140,8 +1229,11 @@
       </c>
       <c r="G27" s="3"/>
       <c r="H27" s="1">
-        <f t="shared" si="0"/>
+        <f>ABS(1-(F27/F28))</f>
         <v>1.9704433497536922E-2</v>
+      </c>
+      <c r="L27">
+        <v>2.6153846153846194E-2</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
@@ -1165,8 +1257,11 @@
       </c>
       <c r="G28" s="3"/>
       <c r="H28" s="1">
-        <f t="shared" si="0"/>
+        <f>ABS(1-(F28/F29))</f>
         <v>1.6694490818029983E-2</v>
+      </c>
+      <c r="L28">
+        <v>2.7227722772277252E-2</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
@@ -1190,8 +1285,11 @@
       </c>
       <c r="G29" s="3"/>
       <c r="H29" s="1">
-        <f t="shared" si="0"/>
+        <f>ABS(1-(F29/F30))</f>
         <v>1.0118043844856706E-2</v>
+      </c>
+      <c r="L29">
+        <v>2.730819245773719E-2</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
@@ -1218,6 +1316,9 @@
         <f>ABS(1-(F30/F31))</f>
         <v>3.130434782608682E-2</v>
       </c>
+      <c r="L30">
+        <v>2.7777777777777901E-2</v>
+      </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31">
@@ -1240,8 +1341,11 @@
       </c>
       <c r="G31" s="3"/>
       <c r="H31" s="1">
-        <f t="shared" si="0"/>
+        <f>ABS(1-(F31/F32))</f>
         <v>7.4766355140186924E-2</v>
+      </c>
+      <c r="L31">
+        <v>2.8571428571428692E-2</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
@@ -1264,11 +1368,14 @@
         <v>53.5</v>
       </c>
       <c r="H32" s="1">
-        <f t="shared" si="0"/>
+        <f>ABS(1-(F32/F33))</f>
         <v>7.4297188755020116E-2</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="L32">
+        <v>2.8907922912205342E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>1988</v>
       </c>
@@ -1288,11 +1395,14 @@
         <v>49.8</v>
       </c>
       <c r="H33" s="1">
-        <f t="shared" si="0"/>
+        <f>ABS(1-(F33/F34))</f>
         <v>7.3275862068965525E-2</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="L33">
+        <v>3.0831099195710587E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>1987</v>
       </c>
@@ -1312,11 +1422,14 @@
         <v>46.4</v>
       </c>
       <c r="H34" s="1">
-        <f t="shared" si="0"/>
+        <f>ABS(1-(F34/F35))</f>
         <v>8.4112149532710401E-2</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="L34">
+        <v>3.130434782608682E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>1986</v>
       </c>
@@ -1336,11 +1449,14 @@
         <v>42.8</v>
       </c>
       <c r="H35" s="1">
-        <f t="shared" si="0"/>
+        <f>ABS(1-(F35/F36))</f>
         <v>9.183673469387732E-2</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="L35">
+        <v>3.1578947368421151E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>1985</v>
       </c>
@@ -1360,11 +1476,15 @@
         <v>39.200000000000003</v>
       </c>
       <c r="H36" s="1">
-        <f t="shared" si="0"/>
+        <f>ABS(1-(F36/F37))</f>
         <v>6.5217391304347894E-2</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J36" s="11"/>
+      <c r="L36">
+        <v>3.2608695652174058E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>1984</v>
       </c>
@@ -1384,61 +1504,78 @@
         <v>36.799999999999997</v>
       </c>
       <c r="H37" s="1">
-        <f t="shared" si="0"/>
+        <f>ABS(1-(F37/F38))</f>
         <v>3.9548022598870025E-2</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="8">
+      <c r="J37" s="11">
+        <f>MAX(H2:H71)</f>
+        <v>0.18181818181818166</v>
+      </c>
+      <c r="L37">
+        <v>3.3298647242455903E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A38" s="7">
         <v>1983</v>
       </c>
-      <c r="B38" s="8">
+      <c r="B38" s="7">
         <v>34.299999999999997</v>
       </c>
-      <c r="C38" s="8">
+      <c r="C38" s="7">
         <v>35</v>
       </c>
-      <c r="D38" s="8">
+      <c r="D38" s="7">
         <v>35.6</v>
       </c>
-      <c r="E38" s="8">
+      <c r="E38" s="7">
         <v>36.5</v>
       </c>
-      <c r="F38" s="8">
+      <c r="F38" s="7">
         <v>35.4</v>
       </c>
-      <c r="G38" s="8"/>
-      <c r="H38" s="9">
-        <f t="shared" si="0"/>
+      <c r="G38" s="7"/>
+      <c r="H38" s="8">
+        <f>ABS(1-(F38/F39))</f>
         <v>0.10280373831775691</v>
       </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="8">
+      <c r="J38" s="11">
+        <f>MIN((H2:H58))</f>
+        <v>2.9985007496251548E-3</v>
+      </c>
+      <c r="L38">
+        <v>3.3707865168539186E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A39" s="7">
         <v>1982</v>
       </c>
-      <c r="B39" s="8">
+      <c r="B39" s="7">
         <v>30.8</v>
       </c>
-      <c r="C39" s="8">
+      <c r="C39" s="7">
         <v>31.5</v>
       </c>
-      <c r="D39" s="8">
+      <c r="D39" s="7">
         <v>32.6</v>
       </c>
-      <c r="E39" s="8">
+      <c r="E39" s="7">
         <v>33.6</v>
       </c>
-      <c r="F39" s="8">
+      <c r="F39" s="7">
         <v>32.1</v>
       </c>
-      <c r="G39" s="8"/>
-      <c r="H39" s="9">
-        <f t="shared" si="0"/>
+      <c r="G39" s="7"/>
+      <c r="H39" s="8">
+        <f>ABS(1-(F39/F40))</f>
         <v>0.11072664359861606</v>
       </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="L39">
+        <v>3.488372093023262E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>1981</v>
       </c>
@@ -1458,36 +1595,42 @@
         <v>28.9</v>
       </c>
       <c r="H40" s="1">
-        <f t="shared" si="0"/>
+        <f>ABS(1-(F40/F41))</f>
         <v>9.4696969696969724E-2</v>
       </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="8">
+      <c r="L40">
+        <v>3.4939759036144658E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A41" s="7">
         <v>1980</v>
       </c>
-      <c r="B41" s="8">
+      <c r="B41" s="7">
         <v>25.4</v>
       </c>
-      <c r="C41" s="8">
+      <c r="C41" s="7">
         <v>26.2</v>
       </c>
-      <c r="D41" s="8">
+      <c r="D41" s="7">
         <v>26.6</v>
       </c>
-      <c r="E41" s="8">
+      <c r="E41" s="7">
         <v>27.2</v>
       </c>
-      <c r="F41" s="8">
+      <c r="F41" s="7">
         <v>26.4</v>
       </c>
-      <c r="G41" s="8"/>
-      <c r="H41" s="9">
-        <f t="shared" si="0"/>
+      <c r="G41" s="7"/>
+      <c r="H41" s="8">
+        <f>ABS(1-(F41/F42))</f>
         <v>0.10460251046025104</v>
       </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="L41">
+        <v>3.7037037037037202E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>1979</v>
       </c>
@@ -1507,11 +1650,14 @@
         <v>23.9</v>
       </c>
       <c r="H42" s="1">
-        <f t="shared" si="0"/>
+        <f>ABS(1-(F42/F43))</f>
         <v>9.1324200913242004E-2</v>
       </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="L42">
+        <v>3.9548022598870025E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>1978</v>
       </c>
@@ -1531,111 +1677,126 @@
         <v>21.9</v>
       </c>
       <c r="H43" s="1">
-        <f t="shared" si="0"/>
+        <f>ABS(1-(F43/F44))</f>
         <v>7.8817733990147687E-2</v>
       </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44" s="8">
+      <c r="L43">
+        <v>4.0540540540540571E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A44" s="7">
         <v>1977</v>
       </c>
-      <c r="B44" s="8">
+      <c r="B44" s="7">
         <v>19.600000000000001</v>
       </c>
-      <c r="C44" s="8">
+      <c r="C44" s="7">
         <v>20.100000000000001</v>
       </c>
-      <c r="D44" s="8">
+      <c r="D44" s="7">
         <v>20.5</v>
       </c>
-      <c r="E44" s="8">
+      <c r="E44" s="7">
         <v>21</v>
       </c>
-      <c r="F44" s="8">
+      <c r="F44" s="7">
         <v>20.3</v>
       </c>
-      <c r="G44" s="8"/>
-      <c r="H44" s="9">
-        <f t="shared" si="0"/>
+      <c r="G44" s="7"/>
+      <c r="H44" s="8">
+        <f>ABS(1-(F44/F45))</f>
         <v>0.12154696132596676</v>
       </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A45" s="8">
+      <c r="L44">
+        <v>4.3356643356643243E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A45" s="7">
         <v>1976</v>
       </c>
-      <c r="B45" s="8">
+      <c r="B45" s="7">
         <v>17.3</v>
       </c>
-      <c r="C45" s="8">
+      <c r="C45" s="7">
         <v>17.7</v>
       </c>
-      <c r="D45" s="8">
+      <c r="D45" s="7">
         <v>18.100000000000001</v>
       </c>
-      <c r="E45" s="8">
+      <c r="E45" s="7">
         <v>19.2</v>
       </c>
-      <c r="F45" s="8">
+      <c r="F45" s="7">
         <v>18.100000000000001</v>
       </c>
-      <c r="G45" s="8"/>
-      <c r="H45" s="9">
-        <f t="shared" si="0"/>
+      <c r="G45" s="7"/>
+      <c r="H45" s="8">
+        <f>ABS(1-(F45/F46))</f>
         <v>0.13125000000000009</v>
       </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A46" s="8">
+      <c r="L45">
+        <v>4.4368600682593851E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A46" s="7">
         <v>1975</v>
       </c>
-      <c r="B46" s="8">
+      <c r="B46" s="7">
         <v>15.3</v>
       </c>
-      <c r="C46" s="8">
+      <c r="C46" s="7">
         <v>15.8</v>
       </c>
-      <c r="D46" s="8">
+      <c r="D46" s="7">
         <v>15.9</v>
       </c>
-      <c r="E46" s="8">
+      <c r="E46" s="7">
         <v>16.8</v>
       </c>
-      <c r="F46" s="8">
+      <c r="F46" s="7">
         <v>16</v>
       </c>
-      <c r="G46" s="8"/>
-      <c r="H46" s="9">
-        <f t="shared" si="0"/>
+      <c r="G46" s="7"/>
+      <c r="H46" s="8">
+        <f>ABS(1-(F46/F47))</f>
         <v>0.15107913669064743</v>
       </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A47" s="8">
+      <c r="L46">
+        <v>4.5321637426900541E-2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A47" s="7">
         <v>1974</v>
       </c>
-      <c r="B47" s="8">
+      <c r="B47" s="7">
         <v>13</v>
       </c>
-      <c r="C47" s="8">
+      <c r="C47" s="7">
         <v>13.5</v>
       </c>
-      <c r="D47" s="8">
+      <c r="D47" s="7">
         <v>14.2</v>
       </c>
-      <c r="E47" s="8">
+      <c r="E47" s="7">
         <v>14.7</v>
       </c>
-      <c r="F47" s="8">
+      <c r="F47" s="7">
         <v>13.9</v>
       </c>
-      <c r="G47" s="8"/>
-      <c r="H47" s="9">
-        <f t="shared" si="0"/>
+      <c r="G47" s="7"/>
+      <c r="H47" s="8">
+        <f>ABS(1-(F47/F48))</f>
         <v>0.15833333333333344</v>
       </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="L47">
+        <v>4.6698872785829293E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>1973</v>
       </c>
@@ -1655,11 +1816,14 @@
         <v>12</v>
       </c>
       <c r="H48" s="1">
-        <f t="shared" si="0"/>
+        <f>ABS(1-(F48/F49))</f>
         <v>9.0909090909090828E-2</v>
       </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="L48">
+        <v>4.9180327868852514E-2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>1972</v>
       </c>
@@ -1679,11 +1843,14 @@
         <v>11</v>
       </c>
       <c r="H49" s="1">
-        <f t="shared" si="0"/>
+        <f>ABS(1-(F49/F50))</f>
         <v>5.7692307692307709E-2</v>
       </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="L49">
+        <v>5.7692307692307709E-2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>1971</v>
       </c>
@@ -1703,11 +1870,14 @@
         <v>10.4</v>
       </c>
       <c r="H50" s="1">
-        <f t="shared" si="0"/>
+        <f>ABS(1-(F50/F51))</f>
         <v>6.1224489795918435E-2</v>
       </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="L50">
+        <v>6.0606060606060552E-2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>1970</v>
       </c>
@@ -1727,11 +1897,14 @@
         <v>9.8000000000000007</v>
       </c>
       <c r="H51" s="1">
-        <f t="shared" si="0"/>
+        <f>ABS(1-(F51/F52))</f>
         <v>3.1578947368421151E-2</v>
       </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="L51">
+        <v>6.1224489795918435E-2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>1969</v>
       </c>
@@ -1751,11 +1924,14 @@
         <v>9.5</v>
       </c>
       <c r="H52" s="1">
-        <f t="shared" si="0"/>
+        <f>ABS(1-(F52/F53))</f>
         <v>3.2608695652174058E-2</v>
       </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="L52">
+        <v>6.5217391304347894E-2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>1968</v>
       </c>
@@ -1775,11 +1951,14 @@
         <v>9.1999999999999993</v>
       </c>
       <c r="H53" s="1">
-        <f t="shared" si="0"/>
+        <f>ABS(1-(F53/F54))</f>
         <v>3.3707865168539186E-2</v>
       </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="L53">
+        <v>7.3275862068965525E-2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>1967</v>
       </c>
@@ -1799,11 +1978,14 @@
         <v>8.9</v>
       </c>
       <c r="H54" s="1">
-        <f t="shared" si="0"/>
+        <f>ABS(1-(F54/F55))</f>
         <v>3.488372093023262E-2</v>
       </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="L54">
+        <v>7.4297188755020116E-2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>1966</v>
       </c>
@@ -1823,11 +2005,14 @@
         <v>8.6</v>
       </c>
       <c r="H55" s="1">
-        <f t="shared" si="0"/>
+        <f>ABS(1-(F55/F56))</f>
         <v>2.3809523809523725E-2</v>
       </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="L55">
+        <v>7.4766355140186924E-2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>1965</v>
       </c>
@@ -1847,11 +2032,14 @@
         <v>8.4</v>
       </c>
       <c r="H56" s="1">
-        <f t="shared" si="0"/>
+        <f>ABS(1-(F56/F57))</f>
         <v>3.7037037037037202E-2</v>
       </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="L56">
+        <v>7.8817733990147687E-2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>1964</v>
       </c>
@@ -1871,11 +2059,14 @@
         <v>8.1</v>
       </c>
       <c r="H57" s="1">
-        <f t="shared" si="0"/>
+        <f>ABS(1-(F57/F58))</f>
         <v>2.5316455696202445E-2</v>
       </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="L57">
+        <v>8.4112149532710401E-2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>1963</v>
       </c>
@@ -1895,11 +2086,14 @@
         <v>7.9</v>
       </c>
       <c r="H58" s="1">
-        <f t="shared" si="0"/>
+        <f>ABS(1-(F58/F59))</f>
         <v>1.2820512820512997E-2</v>
       </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="L58">
+        <v>9.0909090909090828E-2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>1962</v>
       </c>
@@ -1919,11 +2113,14 @@
         <v>7.8</v>
       </c>
       <c r="H59" s="1">
-        <f t="shared" si="0"/>
+        <f>ABS(1-(F59/F60))</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="L59">
+        <v>9.1324200913242004E-2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>1961</v>
       </c>
@@ -1943,11 +2140,14 @@
         <v>7.8</v>
       </c>
       <c r="H60" s="1">
-        <f t="shared" si="0"/>
+        <f>ABS(1-(F60/F61))</f>
         <v>1.298701298701288E-2</v>
       </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="L60">
+        <v>9.183673469387732E-2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>1960</v>
       </c>
@@ -1967,11 +2167,14 @@
         <v>7.7</v>
       </c>
       <c r="H61" s="1">
-        <f t="shared" si="0"/>
+        <f>ABS(1-(F61/F62))</f>
         <v>4.0540540540540571E-2</v>
       </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="L61">
+        <v>9.4696969696969724E-2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>1959</v>
       </c>
@@ -1991,11 +2194,14 @@
         <v>7.4</v>
       </c>
       <c r="H62" s="1">
-        <f t="shared" si="0"/>
+        <f>ABS(1-(F62/F63))</f>
         <v>2.7777777777777901E-2</v>
       </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="L62">
+        <v>0.10000000000000009</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>1958</v>
       </c>
@@ -2015,11 +2221,14 @@
         <v>7.2</v>
       </c>
       <c r="H63" s="1">
-        <f t="shared" si="0"/>
+        <f>ABS(1-(F63/F64))</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="L63">
+        <v>0.10280373831775691</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>1957</v>
       </c>
@@ -2039,11 +2248,14 @@
         <v>7.2</v>
       </c>
       <c r="H64" s="1">
-        <f t="shared" si="0"/>
+        <f>ABS(1-(F64/F65))</f>
         <v>2.8571428571428692E-2</v>
       </c>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="L64">
+        <v>0.10460251046025104</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>1956</v>
       </c>
@@ -2063,11 +2275,14 @@
         <v>7</v>
       </c>
       <c r="H65" s="1">
-        <f t="shared" si="0"/>
+        <f>ABS(1-(F65/F66))</f>
         <v>6.0606060606060552E-2</v>
       </c>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="L65">
+        <v>0.11072664359861606</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>1955</v>
       </c>
@@ -2087,11 +2302,14 @@
         <v>6.6</v>
       </c>
       <c r="H66" s="1">
-        <f t="shared" ref="H66:H72" si="1">ABS(1-(F66/F67))</f>
+        <f>ABS(1-(F66/F67))</f>
         <v>1.538461538461533E-2</v>
       </c>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="L66">
+        <v>0.12154696132596676</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>1954</v>
       </c>
@@ -2111,11 +2329,14 @@
         <v>6.5</v>
       </c>
       <c r="H67" s="1">
-        <f t="shared" si="1"/>
+        <f>ABS(1-(F67/F68))</f>
         <v>1.5625E-2</v>
       </c>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="L67">
+        <v>0.13125000000000009</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>1953</v>
       </c>
@@ -2135,86 +2356,98 @@
         <v>6.4</v>
       </c>
       <c r="H68" s="1">
-        <f t="shared" si="1"/>
+        <f>ABS(1-(F68/F69))</f>
         <v>4.9180327868852514E-2</v>
       </c>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A69" s="8">
+      <c r="L68">
+        <v>0.15107913669064743</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A69" s="7">
         <v>1952</v>
       </c>
-      <c r="B69" s="8">
+      <c r="B69" s="7">
         <v>5.9</v>
       </c>
-      <c r="C69" s="8">
+      <c r="C69" s="7">
         <v>6.1</v>
       </c>
-      <c r="D69" s="8">
+      <c r="D69" s="7">
         <v>6.2</v>
       </c>
-      <c r="E69" s="8">
+      <c r="E69" s="7">
         <v>6.3</v>
       </c>
-      <c r="F69" s="8">
+      <c r="F69" s="7">
         <v>6.1</v>
       </c>
-      <c r="G69" s="8"/>
-      <c r="H69" s="9">
-        <f t="shared" si="1"/>
+      <c r="G69" s="7"/>
+      <c r="H69" s="8">
+        <f>ABS(1-(F69/F70))</f>
         <v>0.17307692307692291</v>
       </c>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A70" s="8">
+      <c r="L69">
+        <v>0.15833333333333344</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A70" s="7">
         <v>1951</v>
       </c>
-      <c r="B70" s="8">
+      <c r="B70" s="7">
         <v>4.8</v>
       </c>
-      <c r="C70" s="8">
+      <c r="C70" s="7">
         <v>5.0999999999999996</v>
       </c>
-      <c r="D70" s="8">
+      <c r="D70" s="7">
         <v>5.3</v>
       </c>
-      <c r="E70" s="8">
+      <c r="E70" s="7">
         <v>5.7</v>
       </c>
-      <c r="F70" s="8">
+      <c r="F70" s="7">
         <v>5.2</v>
       </c>
-      <c r="G70" s="8"/>
-      <c r="H70" s="9">
-        <f t="shared" si="1"/>
+      <c r="G70" s="7"/>
+      <c r="H70" s="8">
+        <f>ABS(1-(F70/F71))</f>
         <v>0.18181818181818166</v>
       </c>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A71" s="8">
+      <c r="L70">
+        <v>0.17307692307692291</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A71" s="7">
         <v>1950</v>
       </c>
-      <c r="B71" s="8">
+      <c r="B71" s="7">
         <v>4.2</v>
       </c>
-      <c r="C71" s="8">
+      <c r="C71" s="7">
         <v>4.3</v>
       </c>
-      <c r="D71" s="8">
+      <c r="D71" s="7">
         <v>4.4000000000000004</v>
       </c>
-      <c r="E71" s="8">
+      <c r="E71" s="7">
         <v>4.5999999999999996</v>
       </c>
-      <c r="F71" s="8">
+      <c r="F71" s="7">
         <v>4.4000000000000004</v>
       </c>
-      <c r="G71" s="8"/>
-      <c r="H71" s="9">
-        <f t="shared" si="1"/>
+      <c r="G71" s="7"/>
+      <c r="H71" s="8">
+        <f>ABS(1-(F71/F72))</f>
         <v>0.10000000000000009</v>
       </c>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="L71">
+        <v>0.18181818181818166</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>1949</v>
       </c>
@@ -2234,7 +2467,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>1948</v>
       </c>
@@ -2248,22 +2481,27 @@
         <v>1.9</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="H74" s="6">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H74" s="5">
         <f>AVERAGE(H2:H37,H40,H42:H43,H48:H68)</f>
         <v>3.6067221898445911E-2</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
       <c r="G75" t="s">
         <v>8</v>
       </c>
-      <c r="H75" s="7">
+      <c r="H75" s="6">
         <f>MEDIAN(H2:H71)</f>
         <v>3.2953671447314981E-2</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="L1:L71" xr:uid="{F8CDEA06-49EE-46B0-8146-D72DB749C91B}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="L2:L71">
+      <sortCondition ref="L1:L71"/>
+    </sortState>
+  </autoFilter>
   <hyperlinks>
     <hyperlink ref="H1" r:id="rId1" xr:uid="{54AE6731-20DB-49CE-B118-26879C7FB911}"/>
   </hyperlinks>

</xml_diff>